<commit_message>
- Add resource quadtree
</commit_message>
<xml_diff>
--- a/CastleVania/Resources/Level/ManagerLevel.xlsx
+++ b/CastleVania/Resources/Level/ManagerLevel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>..\\Resources\\Object\\lv1GO.txt</t>
   </si>
@@ -42,6 +42,18 @@
   </si>
   <si>
     <t>..\\Resources\\Object\\lv2GO.txt</t>
+  </si>
+  <si>
+    <t>..\\Resources\\Map\\lv1QTBG.txt</t>
+  </si>
+  <si>
+    <t>..\\Resources\\Map\\lv2QTBG.txt</t>
+  </si>
+  <si>
+    <t>..\\Resources\\Object\\lv1QTGO.txt</t>
+  </si>
+  <si>
+    <t>..\\Resources\\Object\\lv2QTGO.txt</t>
   </si>
 </sst>
 </file>
@@ -359,10 +371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -370,9 +382,11 @@
     <col min="2" max="2" width="49.5703125" customWidth="1"/>
     <col min="3" max="3" width="51.5703125" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -385,8 +399,14 @@
       <c r="D1" t="s">
         <v>0</v>
       </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -398,6 +418,12 @@
       </c>
       <c r="D2" t="s">
         <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>